<commit_message>
Fixed up some cosmetic issues with silkscreen after reviewing gerbers with Brent @KB1LQD. Fixed an issue I found with the soldermask on pins 1 and 16 of the CC1190 so they used the global setting. Lastly, checked the BOM and pick and place files extensively, optimized for FaradayRF/PCB:NG use. Exported new PDF schematic.
</commit_message>
<xml_diff>
--- a/Kicad-Faraday/OutputFiles/Faraday-REVD(BOM).xlsx
+++ b/Kicad-Faraday/OutputFiles/Faraday-REVD(BOM).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="232">
   <si>
     <t>BTN1</t>
   </si>
@@ -411,9 +411,6 @@
     <t>GRM155R71H222KA01D</t>
   </si>
   <si>
-    <t>LG L29K-F2J1-24-Z</t>
-  </si>
-  <si>
     <t>LQW15AN2N9B00D</t>
   </si>
   <si>
@@ -465,9 +462,6 @@
     <t>10V</t>
   </si>
   <si>
-    <t>LS L29K-G1H2-1-Z</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
@@ -591,9 +585,6 @@
     <t>23K256T-I/STCT-ND</t>
   </si>
   <si>
-    <t>475-3118-1-ND</t>
-  </si>
-  <si>
     <t>627-1054-1-ND</t>
   </si>
   <si>
@@ -606,9 +597,6 @@
     <t>296-36922-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve"> 583-1199-1-ND</t>
-  </si>
-  <si>
     <t>576-3580-1-ND</t>
   </si>
   <si>
@@ -651,9 +639,6 @@
     <t xml:space="preserve">FaradayRF </t>
   </si>
   <si>
-    <t>Assembly Line Items</t>
-  </si>
-  <si>
     <t>Placement Count</t>
   </si>
   <si>
@@ -715,6 +700,21 @@
   </si>
   <si>
     <t>Revision D</t>
+  </si>
+  <si>
+    <t>LG L29K-F2J1-24</t>
+  </si>
+  <si>
+    <t>LS L29K-G1H2-1</t>
+  </si>
+  <si>
+    <t>475-1193-1-ND</t>
+  </si>
+  <si>
+    <t>583-1199-1-ND</t>
+  </si>
+  <si>
+    <t>SMT Line Items</t>
   </si>
 </sst>
 </file>
@@ -1345,14 +1345,14 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="17" xfId="27" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="26" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="25" borderId="0" xfId="34" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="25" borderId="0" xfId="34" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="26" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1711,41 +1711,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B61"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.46484375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.59765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>231</v>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>226</v>
       </c>
       <c r="D1" s="11">
-        <v>42692</v>
+        <v>42694</v>
       </c>
       <c r="E1" s="12"/>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>118</v>
       </c>
@@ -1762,14 +1762,14 @@
         <v>124</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G2" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="G2" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="H2" s="22"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1783,15 +1783,15 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>123</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>5</v>
@@ -1817,7 +1817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>125</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>5</v>
@@ -1843,7 +1843,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>126</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>5</v>
@@ -1869,7 +1869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
@@ -1886,7 +1886,7 @@
         <v>127</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>5</v>
@@ -1895,7 +1895,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>128</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>5</v>
@@ -1921,7 +1921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1935,10 +1935,10 @@
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>5</v>
@@ -1947,7 +1947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>129</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>5</v>
@@ -1973,7 +1973,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1981,25 +1981,25 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -2013,19 +2013,19 @@
         <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -2033,25 +2033,25 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -2059,25 +2059,25 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -2091,19 +2091,19 @@
         <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -2111,15 +2111,18 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E16" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -2127,15 +2130,18 @@
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -2143,21 +2149,21 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>130</v>
+        <v>227</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>190</v>
+        <v>229</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -2165,21 +2171,21 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>148</v>
+        <v>228</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2192,10 +2198,13 @@
       <c r="D20" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -2209,15 +2218,15 @@
         <v>36</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -2231,15 +2240,15 @@
         <v>36</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
@@ -2253,15 +2262,15 @@
         <v>36</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -2275,15 +2284,15 @@
         <v>36</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -2294,18 +2303,18 @@
         <v>44</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
@@ -2313,18 +2322,18 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
@@ -2332,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>36</v>
@@ -2341,12 +2350,12 @@
         <v>48</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -2359,10 +2368,13 @@
       <c r="D28" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="E28" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>22232021</v>
       </c>
@@ -2379,12 +2391,12 @@
         <v>22232021</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
@@ -2401,12 +2413,12 @@
         <v>54</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -2417,15 +2429,18 @@
         <v>55</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>56</v>
       </c>
@@ -2442,12 +2457,12 @@
         <v>58</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -2460,10 +2475,13 @@
       <c r="D33" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="E33" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -2476,10 +2494,13 @@
       <c r="D34" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="E34" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
@@ -2492,10 +2513,13 @@
       <c r="D35" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="E35" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -2508,10 +2532,13 @@
       <c r="D36" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="E36" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>67</v>
       </c>
@@ -2528,12 +2555,12 @@
         <v>67</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>70</v>
       </c>
@@ -2541,7 +2568,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>69</v>
@@ -2550,12 +2577,12 @@
         <v>70</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>360</v>
       </c>
@@ -2563,23 +2590,23 @@
         <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G39" s="6">
         <v>0.01</v>
       </c>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
@@ -2587,23 +2614,23 @@
         <v>2</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G40" s="6">
         <v>0.01</v>
       </c>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>73</v>
       </c>
@@ -2611,23 +2638,23 @@
         <v>8</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G41" s="6">
         <v>0.01</v>
       </c>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>74</v>
       </c>
@@ -2635,23 +2662,23 @@
         <v>2</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G42" s="6">
         <v>0.01</v>
       </c>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
@@ -2659,23 +2686,23 @@
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G43" s="6">
         <v>0.01</v>
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>76</v>
       </c>
@@ -2689,17 +2716,17 @@
         <v>71</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G44" s="6">
         <v>0.01</v>
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>29</v>
       </c>
@@ -2707,17 +2734,19 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F45" s="1"/>
       <c r="G45" s="6"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -2730,10 +2759,13 @@
       <c r="D46" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="E46" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>80</v>
       </c>
@@ -2750,12 +2782,12 @@
         <v>80</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>83</v>
       </c>
@@ -2777,7 +2809,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>85</v>
       </c>
@@ -2794,12 +2826,12 @@
         <v>85</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>87</v>
       </c>
@@ -2816,12 +2848,12 @@
         <v>87</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>90</v>
       </c>
@@ -2835,15 +2867,15 @@
         <v>92</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>93</v>
       </c>
@@ -2857,15 +2889,15 @@
         <v>95</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>96</v>
       </c>
@@ -2879,15 +2911,15 @@
         <v>98</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>99</v>
       </c>
@@ -2904,12 +2936,12 @@
         <v>99</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>195</v>
+        <v>230</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>29</v>
       </c>
@@ -2926,12 +2958,12 @@
         <v>101</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>104</v>
       </c>
@@ -2945,15 +2977,15 @@
         <v>106</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>107</v>
       </c>
@@ -2970,12 +3002,12 @@
         <v>107</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>109</v>
       </c>
@@ -2992,12 +3024,12 @@
         <v>109</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>111</v>
       </c>
@@ -3014,12 +3046,12 @@
         <v>111</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>114</v>
       </c>
@@ -3036,12 +3068,12 @@
         <v>114</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>116</v>
       </c>
@@ -3058,34 +3090,34 @@
         <v>116</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="C62" s="4"/>
       <c r="D62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E63"/>
       <c r="F63"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
         <f>COUNTA(A3:A61)-COUNTA(A3,A16,A17,A20,A28,A31,A33,A34,A35,A36,A29,A45,A46,A55)</f>
         <v>45</v>
@@ -3095,7 +3127,7 @@
         <v>90</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D64"/>
       <c r="E64" s="1"/>
@@ -3103,14 +3135,14 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="19"/>
       <c r="B65" s="20">
         <f>SUM(B32,B29)</f>
         <v>3</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to pick and place file to remove comment plus removed erroneous flash chip from BOM
</commit_message>
<xml_diff>
--- a/Kicad-Faraday/OutputFiles/Faraday-REVD(BOM).xlsx
+++ b/Kicad-Faraday/OutputFiles/Faraday-REVD(BOM).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="231">
   <si>
     <t>BTN1</t>
   </si>
@@ -322,9 +322,6 @@
   </si>
   <si>
     <t>U5</t>
-  </si>
-  <si>
-    <t>IS25LQ080-JNLE-TR</t>
   </si>
   <si>
     <t>U9</t>
@@ -1711,8 +1708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,13 +1726,13 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D1" s="11">
         <v>42694</v>
@@ -1747,25 +1744,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="24" t="s">
         <v>121</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>122</v>
       </c>
       <c r="H2" s="24"/>
     </row>
@@ -1783,10 +1780,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1805,10 +1802,10 @@
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>5</v>
@@ -1831,10 +1828,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>5</v>
@@ -1857,10 +1854,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>5</v>
@@ -1877,16 +1874,16 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>5</v>
@@ -1909,10 +1906,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>5</v>
@@ -1935,10 +1932,10 @@
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>5</v>
@@ -1961,10 +1958,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>5</v>
@@ -1981,22 +1978,22 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2013,16 +2010,16 @@
         <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2033,22 +2030,22 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2059,22 +2056,22 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2091,16 +2088,16 @@
         <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2111,7 +2108,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>4</v>
@@ -2130,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>21</v>
@@ -2149,16 +2146,16 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -2171,16 +2168,16 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2218,10 +2215,10 @@
         <v>36</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -2240,10 +2237,10 @@
         <v>36</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -2262,10 +2259,10 @@
         <v>36</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2284,10 +2281,10 @@
         <v>36</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -2303,13 +2300,13 @@
         <v>44</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -2322,13 +2319,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2341,7 +2338,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>36</v>
@@ -2350,7 +2347,7 @@
         <v>48</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2391,7 +2388,7 @@
         <v>22232021</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2413,7 +2410,7 @@
         <v>54</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -2429,13 +2426,13 @@
         <v>55</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2457,7 +2454,7 @@
         <v>58</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2555,7 +2552,7 @@
         <v>67</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2568,7 +2565,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>69</v>
@@ -2577,7 +2574,7 @@
         <v>70</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -2590,16 +2587,16 @@
         <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G39" s="6">
         <v>0.01</v>
@@ -2614,16 +2611,16 @@
         <v>2</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G40" s="6">
         <v>0.01</v>
@@ -2638,16 +2635,16 @@
         <v>8</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G41" s="6">
         <v>0.01</v>
@@ -2662,16 +2659,16 @@
         <v>2</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G42" s="6">
         <v>0.01</v>
@@ -2686,16 +2683,16 @@
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G43" s="6">
         <v>0.01</v>
@@ -2716,10 +2713,10 @@
         <v>71</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G44" s="6">
         <v>0.01</v>
@@ -2734,7 +2731,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>71</v>
@@ -2782,7 +2779,7 @@
         <v>80</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -2826,7 +2823,7 @@
         <v>85</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -2848,7 +2845,7 @@
         <v>87</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -2867,10 +2864,10 @@
         <v>92</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -2889,10 +2886,10 @@
         <v>95</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -2911,10 +2908,10 @@
         <v>98</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -2936,7 +2933,7 @@
         <v>99</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -2949,148 +2946,148 @@
         <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E55" s="1" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="3">
-        <v>1</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="E56" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="3">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="D57" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="F57" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="3">
-        <v>1</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="D58" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="3">
-        <v>1</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="E59" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B60" s="3">
-        <v>1</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="D60" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B61" s="3">
         <v>2</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -3104,13 +3101,13 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E63"/>
       <c r="F63"/>
@@ -3127,7 +3124,7 @@
         <v>90</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D64"/>
       <c r="E64" s="1"/>
@@ -3142,7 +3139,7 @@
         <v>3</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>